<commit_message>
new names cool IV fluid play i guess
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minhv\OneDrive\Documents\GitHub\diploma\modelz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9B390B-AFC7-42A4-B5AF-75E42A28A5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794CDCEF-A947-4CAF-A09E-6D8DB00BAA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{95705682-6DEC-4651-AA93-826AF7011AAB}"/>
+    <workbookView xWindow="23040" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{95705682-6DEC-4651-AA93-826AF7011AAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>Stock Name</t>
   </si>
@@ -279,6 +279,15 @@
   </si>
   <si>
     <t>ICU Medical</t>
+  </si>
+  <si>
+    <t>&lt;35</t>
+  </si>
+  <si>
+    <t>&lt;8</t>
+  </si>
+  <si>
+    <t>Ferroglobe</t>
   </si>
 </sst>
 </file>
@@ -288,7 +297,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +305,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -399,7 +415,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -450,6 +466,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -787,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A47BAB04-299C-4B1D-A1B7-A616FD6A37A4}">
-  <dimension ref="B1:U58"/>
+  <dimension ref="B1:U59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -936,16 +958,35 @@
       <c r="B4" t="s">
         <v>25</v>
       </c>
+      <c r="C4" s="8">
+        <v>55.35</v>
+      </c>
+      <c r="D4" s="9">
+        <f>+C4*0.85</f>
+        <v>47.047499999999999</v>
+      </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>26</v>
       </c>
+      <c r="C5" s="8">
+        <v>234.96</v>
+      </c>
+      <c r="D5" s="9">
+        <v>200</v>
+      </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>27</v>
       </c>
+      <c r="C6" s="8">
+        <v>496.29</v>
+      </c>
+      <c r="D6" s="9">
+        <v>307.69979999999998</v>
+      </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
@@ -988,6 +1029,12 @@
       <c r="B13" t="s">
         <v>33</v>
       </c>
+      <c r="C13" s="8">
+        <v>720</v>
+      </c>
+      <c r="D13" s="9">
+        <v>200</v>
+      </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
@@ -1173,6 +1220,7 @@
       <c r="B45" t="s">
         <v>66</v>
       </c>
+      <c r="D45" s="19"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
@@ -1198,6 +1246,9 @@
       <c r="B50" t="s">
         <v>71</v>
       </c>
+      <c r="C50" s="8">
+        <v>171.72</v>
+      </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
@@ -1218,6 +1269,12 @@
       <c r="B54" t="s">
         <v>75</v>
       </c>
+      <c r="C54" s="8">
+        <v>8.4</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
@@ -1227,8 +1284,7 @@
         <v>219.85</v>
       </c>
       <c r="D55" s="9">
-        <f>+C55/1.38</f>
-        <v>159.31159420289856</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
@@ -1247,11 +1303,29 @@
       <c r="B57" t="s">
         <v>79</v>
       </c>
+      <c r="C57" s="8">
+        <v>36.549999999999997</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>80</v>
       </c>
+      <c r="C58" s="8">
+        <v>183.05</v>
+      </c>
+      <c r="D58" s="8">
+        <v>54.863725490196096</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>83</v>
+      </c>
+      <c r="D59" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>